<commit_message>
bio & lexicon completed
</commit_message>
<xml_diff>
--- a/TestData/Backend_data.xlsx
+++ b/TestData/Backend_data.xlsx
@@ -14,12 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>testCaseID</t>
   </si>
   <si>
+    <t>Lexican</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>Connector1</t>
+  </si>
+  <si>
+    <t>Predicate</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>predicate_designation</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t>testCaseID_01</t>
+  </si>
+  <si>
+    <t>Jack_test</t>
+  </si>
+  <si>
+    <t>Concrete_test</t>
+  </si>
+  <si>
+    <t>11 - a</t>
+  </si>
+  <si>
+    <t>34 - is the</t>
+  </si>
+  <si>
+    <t>2 - pure setting</t>
+  </si>
+  <si>
+    <t>9 - bridge</t>
+  </si>
+  <si>
+    <t>Algebra</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Calculation</t>
   </si>
 </sst>
 </file>
@@ -32,7 +89,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,10 +106,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Consolas"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -508,155 +569,167 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,25 +1049,92 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="17.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="10.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="14.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="14.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="27.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="13.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="11.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:11">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>